<commit_message>
make r.yos effective and more analysis on demographics
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/RunControl_M2.1_new.xlsx
+++ b/IO_M2.1_new/RunControl_M2.1_new.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="373">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1181,6 +1181,12 @@
   </si>
   <si>
     <t>save.indiv</t>
+  </si>
+  <si>
+    <t>D1F075-mature1_lowB</t>
+  </si>
+  <si>
+    <t>D1F075-mature1_gn1_lowB</t>
   </si>
 </sst>
 </file>
@@ -2145,10 +2151,10 @@
   <dimension ref="A1:AY58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15:C24"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,7 +3246,7 @@
         <v>294</v>
       </c>
       <c r="C14" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="45" t="b">
         <v>1</v>
@@ -3395,7 +3401,7 @@
         <v>294</v>
       </c>
       <c r="C15" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="45" t="b">
         <v>1</v>
@@ -3550,7 +3556,7 @@
         <v>294</v>
       </c>
       <c r="C16" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="45" t="b">
         <v>1</v>
@@ -3705,7 +3711,7 @@
         <v>294</v>
       </c>
       <c r="C17" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="45" t="b">
         <v>1</v>
@@ -3860,7 +3866,7 @@
         <v>294</v>
       </c>
       <c r="C18" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="45" t="b">
         <v>1</v>
@@ -4015,7 +4021,7 @@
         <v>302</v>
       </c>
       <c r="C19" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="45" t="b">
         <v>1</v>
@@ -4170,7 +4176,7 @@
         <v>302</v>
       </c>
       <c r="C20" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="45" t="b">
         <v>1</v>
@@ -4325,7 +4331,7 @@
         <v>302</v>
       </c>
       <c r="C21" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="45" t="b">
         <v>1</v>
@@ -4480,7 +4486,7 @@
         <v>302</v>
       </c>
       <c r="C22" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="45" t="b">
         <v>1</v>
@@ -4635,7 +4641,7 @@
         <v>302</v>
       </c>
       <c r="C23" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="45" t="b">
         <v>1</v>
@@ -4790,7 +4796,7 @@
         <v>302</v>
       </c>
       <c r="C24" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="45" t="b">
         <v>1</v>
@@ -4967,62 +4973,314 @@
       <c r="AY25" s="48"/>
     </row>
     <row r="26" spans="1:51" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="49"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="52"/>
-      <c r="AF26" s="51"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AN26" s="44"/>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="47"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="46"/>
-      <c r="AU26" s="46"/>
-      <c r="AV26" s="46"/>
-      <c r="AW26" s="48"/>
-      <c r="AX26" s="48"/>
-      <c r="AY26" s="48"/>
+      <c r="A26" s="34" t="s">
+        <v>371</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="C26" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G26" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="43">
+        <v>600</v>
+      </c>
+      <c r="I26" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="K26" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="L26" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="M26" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="N26" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26" s="51">
+        <v>0</v>
+      </c>
+      <c r="P26" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="51">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="R26" s="43">
+        <v>3</v>
+      </c>
+      <c r="S26" s="43">
+        <v>75</v>
+      </c>
+      <c r="T26" s="43">
+        <v>50</v>
+      </c>
+      <c r="U26" s="43">
+        <v>60</v>
+      </c>
+      <c r="V26" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="W26" s="43">
+        <v>0</v>
+      </c>
+      <c r="X26" s="43">
+        <v>10</v>
+      </c>
+      <c r="Y26" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="Z26" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="AA26" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="AB26" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="AC26" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AD26" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE26" s="52">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AF26" s="51">
+        <v>0.12</v>
+      </c>
+      <c r="AG26" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH26" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI26" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="AJ26" s="43">
+        <v>30</v>
+      </c>
+      <c r="AK26" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL26" s="43">
+        <v>5</v>
+      </c>
+      <c r="AM26" s="43">
+        <v>200</v>
+      </c>
+      <c r="AN26" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO26" s="43">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="AQ26" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="AR26" s="43">
+        <v>200</v>
+      </c>
+      <c r="AS26" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT26" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="AU26" s="46">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AV26" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="AW26" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY26" s="48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:51" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="49"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="51"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="51"/>
-      <c r="AD27" s="51"/>
-      <c r="AE27" s="52"/>
-      <c r="AF27" s="51"/>
-      <c r="AH27" s="44"/>
-      <c r="AI27" s="44"/>
-      <c r="AN27" s="44"/>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="47"/>
-      <c r="AS27" s="44"/>
-      <c r="AT27" s="46"/>
-      <c r="AU27" s="46"/>
-      <c r="AV27" s="46"/>
-      <c r="AW27" s="48"/>
-      <c r="AX27" s="48"/>
-      <c r="AY27" s="48"/>
+      <c r="A27" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="C27" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="43">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="43">
+        <v>600</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="J27" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="L27" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="M27" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="N27" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="O27" s="51">
+        <v>-0.01</v>
+      </c>
+      <c r="P27" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="51">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="R27" s="43">
+        <v>3</v>
+      </c>
+      <c r="S27" s="43">
+        <v>75</v>
+      </c>
+      <c r="T27" s="43">
+        <v>50</v>
+      </c>
+      <c r="U27" s="43">
+        <v>60</v>
+      </c>
+      <c r="V27" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="W27" s="43">
+        <v>0</v>
+      </c>
+      <c r="X27" s="43">
+        <v>10</v>
+      </c>
+      <c r="Y27" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="Z27" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="AA27" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="AB27" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="AC27" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AD27" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE27" s="52">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AF27" s="51">
+        <v>0.12</v>
+      </c>
+      <c r="AG27" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH27" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI27" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="AJ27" s="43">
+        <v>30</v>
+      </c>
+      <c r="AK27" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL27" s="43">
+        <v>5</v>
+      </c>
+      <c r="AM27" s="43">
+        <v>200</v>
+      </c>
+      <c r="AN27" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO27" s="43">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="AQ27" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="AR27" s="43">
+        <v>200</v>
+      </c>
+      <c r="AS27" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT27" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="AU27" s="46">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AV27" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="AW27" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX27" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY27" s="48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:51" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="49"/>
@@ -7886,7 +8144,7 @@
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AB6:AB9 V6:V9 AB13:AB51 V13:V51">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AB6:AB9 V6:V9 V13:V51 AB13:AB51">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
@@ -7894,7 +8152,7 @@
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="Y6:AA9 AC6:AC9 AE6:AE9 AC48:AC51 AC13:AC42 Y13:AA51 AE13:AE51">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="Y6:AA9 AC6:AC9 AE6:AE9 AC48:AC51 AE13:AE51 Y13:AA51 AC13:AC42">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
More analysis for M2.1
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/RunControl_M2.1_new.xlsx
+++ b/IO_M2.1_new/RunControl_M2.1_new.xlsx
@@ -31,6 +31,7 @@
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1459,10 +1460,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1471,13 +1469,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2151,10 +2152,10 @@
   <dimension ref="A1:AY58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29:D30"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,62 +2351,62 @@
       </c>
     </row>
     <row r="4" spans="1:51" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="54"/>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="56"/>
+      <c r="F4" s="60"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="57" t="s">
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="57"/>
+      <c r="M4" s="56"/>
       <c r="N4" s="28"/>
-      <c r="O4" s="58" t="s">
+      <c r="O4" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="57" t="s">
+      <c r="P4" s="57"/>
+      <c r="Q4" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
       <c r="Y4" s="29"/>
       <c r="Z4" s="29"/>
-      <c r="AA4" s="58" t="s">
+      <c r="AA4" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="60" t="s">
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="60"/>
-      <c r="AF4" s="60"/>
+      <c r="AE4" s="55"/>
+      <c r="AF4" s="55"/>
       <c r="AG4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH4" s="55" t="s">
+      <c r="AH4" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="AI4" s="55"/>
-      <c r="AJ4" s="55"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
       <c r="AK4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2413,17 +2414,17 @@
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
       <c r="AO4" s="21"/>
-      <c r="AP4" s="60" t="s">
+      <c r="AP4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="60"/>
-      <c r="AS4" s="61" t="s">
+      <c r="AQ4" s="55"/>
+      <c r="AR4" s="55"/>
+      <c r="AS4" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="AT4" s="61"/>
-      <c r="AU4" s="61"/>
-      <c r="AV4" s="61"/>
+      <c r="AT4" s="59"/>
+      <c r="AU4" s="59"/>
+      <c r="AV4" s="59"/>
       <c r="AW4" s="15"/>
       <c r="AX4" s="22"/>
       <c r="AY4" s="20"/>
@@ -3246,7 +3247,7 @@
         <v>294</v>
       </c>
       <c r="C14" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="45" t="b">
         <v>1</v>
@@ -3401,7 +3402,7 @@
         <v>294</v>
       </c>
       <c r="C15" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="45" t="b">
         <v>1</v>
@@ -3556,7 +3557,7 @@
         <v>294</v>
       </c>
       <c r="C16" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="45" t="b">
         <v>1</v>
@@ -3711,7 +3712,7 @@
         <v>294</v>
       </c>
       <c r="C17" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="45" t="b">
         <v>1</v>
@@ -3866,7 +3867,7 @@
         <v>294</v>
       </c>
       <c r="C18" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="45" t="b">
         <v>1</v>
@@ -4021,7 +4022,7 @@
         <v>302</v>
       </c>
       <c r="C19" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="45" t="b">
         <v>1</v>
@@ -4176,7 +4177,7 @@
         <v>302</v>
       </c>
       <c r="C20" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="45" t="b">
         <v>1</v>
@@ -4331,7 +4332,7 @@
         <v>302</v>
       </c>
       <c r="C21" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="45" t="b">
         <v>1</v>
@@ -4486,7 +4487,7 @@
         <v>302</v>
       </c>
       <c r="C22" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="45" t="b">
         <v>1</v>
@@ -4641,7 +4642,7 @@
         <v>302</v>
       </c>
       <c r="C23" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="45" t="b">
         <v>1</v>
@@ -4796,7 +4797,7 @@
         <v>302</v>
       </c>
       <c r="C24" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="45" t="b">
         <v>1</v>
@@ -4980,7 +4981,7 @@
         <v>302</v>
       </c>
       <c r="C26" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="45" t="b">
         <v>0</v>
@@ -5135,7 +5136,7 @@
         <v>302</v>
       </c>
       <c r="C27" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="45" t="b">
         <v>0</v>
@@ -5379,9 +5380,11 @@
         <v>320</v>
       </c>
       <c r="C31" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D31" s="45"/>
       <c r="E31" t="s">
         <v>211</v>
       </c>
@@ -5532,9 +5535,11 @@
         <v>322</v>
       </c>
       <c r="C32" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D32" s="45"/>
       <c r="E32" t="s">
         <v>211</v>
       </c>
@@ -5685,9 +5690,11 @@
         <v>324</v>
       </c>
       <c r="C33" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D33" s="45"/>
       <c r="E33" t="s">
         <v>211</v>
       </c>
@@ -5838,9 +5845,11 @@
         <v>326</v>
       </c>
       <c r="C34" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D34" s="45"/>
       <c r="E34" t="s">
         <v>211</v>
       </c>
@@ -5991,9 +6000,11 @@
         <v>328</v>
       </c>
       <c r="C35" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="45"/>
       <c r="E35" t="s">
         <v>211</v>
       </c>
@@ -6173,9 +6184,11 @@
         <v>331</v>
       </c>
       <c r="C37" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D37" s="45"/>
       <c r="E37" t="s">
         <v>211</v>
       </c>
@@ -6326,9 +6339,11 @@
         <v>333</v>
       </c>
       <c r="C38" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D38" s="45"/>
       <c r="E38" t="s">
         <v>211</v>
       </c>
@@ -6479,9 +6494,11 @@
         <v>335</v>
       </c>
       <c r="C39" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D39" s="45"/>
       <c r="E39" t="s">
         <v>211</v>
       </c>
@@ -6632,9 +6649,11 @@
         <v>337</v>
       </c>
       <c r="C40" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D40" s="45"/>
       <c r="E40" t="s">
         <v>211</v>
       </c>
@@ -6785,9 +6804,11 @@
         <v>339</v>
       </c>
       <c r="C41" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D41" s="45"/>
       <c r="E41" t="s">
         <v>211</v>
       </c>
@@ -6967,9 +6988,11 @@
         <v>356</v>
       </c>
       <c r="C43" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D43" s="45"/>
       <c r="E43" t="s">
         <v>211</v>
       </c>
@@ -7121,9 +7144,11 @@
         <v>357</v>
       </c>
       <c r="C44" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D44" s="45"/>
       <c r="E44" t="s">
         <v>211</v>
       </c>
@@ -7275,9 +7300,11 @@
         <v>358</v>
       </c>
       <c r="C45" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D45" s="45"/>
       <c r="E45" t="s">
         <v>211</v>
       </c>
@@ -7429,9 +7456,11 @@
         <v>359</v>
       </c>
       <c r="C46" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D46" s="45"/>
       <c r="E46" t="s">
         <v>211</v>
       </c>
@@ -7583,9 +7612,11 @@
         <v>360</v>
       </c>
       <c r="C47" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D47" s="45"/>
       <c r="E47" t="s">
         <v>211</v>
       </c>
@@ -7796,9 +7827,11 @@
         <v>353</v>
       </c>
       <c r="C50" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D50" s="45"/>
       <c r="E50" t="s">
         <v>211</v>
       </c>
@@ -7949,9 +7982,11 @@
         <v>354</v>
       </c>
       <c r="C51" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="45" t="b">
         <v>0</v>
       </c>
-      <c r="D51" s="45"/>
       <c r="E51" t="s">
         <v>211</v>
       </c>
@@ -8111,17 +8146,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I4:K4"/>
     <mergeCell ref="AP4:AR4"/>
     <mergeCell ref="Q4:X4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AH4:AJ4"/>
     <mergeCell ref="AS4:AV4"/>
     <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN51">

</xml_diff>

<commit_message>
Graphs for forward looking scenario in M2.1b
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/RunControl_M2.1_new.xlsx
+++ b/IO_M2.1_new/RunControl_M2.1_new.xlsx
@@ -2055,7 +2055,10 @@
     <xf numFmtId="2" fontId="16" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2064,16 +2067,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5224,10 +5224,10 @@
   <dimension ref="A1:AY112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AC18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AD21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD38"/>
+      <selection pane="bottomRight" activeCell="AI45" sqref="AI45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5423,62 +5423,62 @@
       </c>
     </row>
     <row r="4" spans="1:51" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="120"/>
+      <c r="F4" s="116"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="116" t="s">
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="116"/>
+      <c r="M4" s="117"/>
       <c r="N4" s="28"/>
-      <c r="O4" s="117" t="s">
+      <c r="O4" s="118" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="116" t="s">
+      <c r="P4" s="118"/>
+      <c r="Q4" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
-      <c r="T4" s="116"/>
-      <c r="U4" s="116"/>
-      <c r="V4" s="116"/>
-      <c r="W4" s="116"/>
-      <c r="X4" s="116"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
+      <c r="V4" s="117"/>
+      <c r="W4" s="117"/>
+      <c r="X4" s="117"/>
       <c r="Y4" s="29"/>
       <c r="Z4" s="29"/>
-      <c r="AA4" s="117" t="s">
+      <c r="AA4" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="AB4" s="117"/>
-      <c r="AC4" s="117"/>
-      <c r="AD4" s="115" t="s">
+      <c r="AB4" s="118"/>
+      <c r="AC4" s="118"/>
+      <c r="AD4" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="115"/>
+      <c r="AE4" s="120"/>
+      <c r="AF4" s="120"/>
       <c r="AG4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH4" s="118" t="s">
+      <c r="AH4" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="AI4" s="118"/>
-      <c r="AJ4" s="118"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="115"/>
       <c r="AK4" s="21" t="s">
         <v>70</v>
       </c>
@@ -5486,17 +5486,17 @@
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
       <c r="AO4" s="21"/>
-      <c r="AP4" s="115" t="s">
+      <c r="AP4" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="AQ4" s="115"/>
-      <c r="AR4" s="115"/>
-      <c r="AS4" s="119" t="s">
+      <c r="AQ4" s="120"/>
+      <c r="AR4" s="120"/>
+      <c r="AS4" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="AT4" s="119"/>
-      <c r="AU4" s="119"/>
-      <c r="AV4" s="119"/>
+      <c r="AT4" s="121"/>
+      <c r="AU4" s="121"/>
+      <c r="AV4" s="121"/>
       <c r="AW4" s="15"/>
       <c r="AX4" s="22"/>
       <c r="AY4" s="20"/>
@@ -9639,7 +9639,7 @@
         <v>342</v>
       </c>
       <c r="AJ38" s="65">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AK38" s="65" t="s">
         <v>115</v>
@@ -18741,17 +18741,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I4:K4"/>
     <mergeCell ref="AP4:AR4"/>
     <mergeCell ref="Q4:X4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AH4:AJ4"/>
     <mergeCell ref="AS4:AV4"/>
     <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <dataValidations xWindow="1269" yWindow="762" count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN108:AN112 AN13:AN105">

</xml_diff>

<commit_message>
update script for Gang
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/RunControl_M2.1_new.xlsx
+++ b/IO_M2.1_new/RunControl_M2.1_new.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_Main\IO_M2.1_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="503">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1589,6 +1589,9 @@
   </si>
   <si>
     <t>75% initial Funding; DC 3.5; ir 3.52,    SD 1.77%  (Lower discount rate)</t>
+  </si>
+  <si>
+    <t>D1F075-average_steady</t>
   </si>
 </sst>
 </file>
@@ -2187,7 +2190,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3529,9 +3538,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625"/>
-    <col min="2" max="2" width="16.75"/>
-    <col min="3" max="1025" width="8.625"/>
+    <col min="1" max="1" width="7.5703125"/>
+    <col min="2" max="2" width="16.7109375"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3589,17 +3598,17 @@
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="14" style="42" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="14.375" customWidth="1"/>
-    <col min="8" max="8" width="12.875" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="42" customWidth="1"/>
-    <col min="10" max="10" width="13.125" customWidth="1"/>
-    <col min="12" max="12" width="11.875" customWidth="1"/>
-    <col min="13" max="13" width="18.875" customWidth="1"/>
-    <col min="14" max="14" width="15.75" customWidth="1"/>
-    <col min="15" max="15" width="14.875" customWidth="1"/>
-    <col min="16" max="16" width="14.25" style="42" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="42" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -4547,12 +4556,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.625" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="7" width="9.375" style="77" customWidth="1"/>
-    <col min="8" max="8" width="11.75" style="77" customWidth="1"/>
-    <col min="9" max="9" width="10.625" style="77" customWidth="1"/>
-    <col min="10" max="10" width="10.25" style="77" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9.42578125" style="77" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="77" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="77" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="77" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -5143,7 +5152,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.625"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -5224,10 +5233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY109"/>
+  <dimension ref="A1:AY111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="N99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="A111" sqref="A111"/>
@@ -5235,34 +5244,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.625" customWidth="1"/>
-    <col min="2" max="2" width="84.625" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="42" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="42" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="20.25" customWidth="1"/>
-    <col min="7" max="7" width="9.125" customWidth="1"/>
-    <col min="8" max="8" width="8.25" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
     <col min="9" max="10" width="16" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="20.875" customWidth="1"/>
-    <col min="12" max="12" width="24.375"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125"/>
     <col min="13" max="14" width="22" customWidth="1"/>
-    <col min="15" max="16" width="13.125" customWidth="1"/>
-    <col min="17" max="21" width="9.25" customWidth="1"/>
+    <col min="15" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="21" width="9.28515625" customWidth="1"/>
     <col min="22" max="22" width="16"/>
-    <col min="23" max="24" width="12.75"/>
-    <col min="25" max="26" width="10.875" customWidth="1"/>
-    <col min="27" max="29" width="12.75"/>
-    <col min="30" max="30" width="11.125" customWidth="1"/>
-    <col min="31" max="31" width="12.75" style="24"/>
-    <col min="32" max="35" width="12.75"/>
-    <col min="36" max="36" width="12.75" customWidth="1"/>
-    <col min="37" max="37" width="11.875" customWidth="1"/>
-    <col min="42" max="43" width="11.75" customWidth="1"/>
-    <col min="44" max="44" width="13.125" customWidth="1"/>
-    <col min="45" max="48" width="12.75"/>
+    <col min="23" max="24" width="12.7109375"/>
+    <col min="25" max="26" width="10.85546875" customWidth="1"/>
+    <col min="27" max="29" width="12.7109375"/>
+    <col min="30" max="30" width="11.140625" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="24"/>
+    <col min="32" max="35" width="12.7109375"/>
+    <col min="36" max="36" width="12.7109375" customWidth="1"/>
+    <col min="37" max="37" width="11.85546875" customWidth="1"/>
+    <col min="42" max="43" width="11.7109375" customWidth="1"/>
+    <col min="44" max="44" width="13.140625" customWidth="1"/>
+    <col min="45" max="48" width="12.7109375"/>
     <col min="51" max="51" width="9" customWidth="1"/>
-    <col min="52" max="1038" width="8.625"/>
+    <col min="52" max="1038" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.25">
@@ -6313,161 +6322,6 @@
       <c r="AW13" s="18"/>
       <c r="AX13" s="18"/>
       <c r="AY13" s="18"/>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="C14" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>207</v>
-      </c>
-      <c r="F14" t="s">
-        <v>184</v>
-      </c>
-      <c r="G14">
-        <v>1000</v>
-      </c>
-      <c r="H14">
-        <v>500</v>
-      </c>
-      <c r="I14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" t="s">
-        <v>109</v>
-      </c>
-      <c r="K14" t="s">
-        <v>204</v>
-      </c>
-      <c r="L14" t="s">
-        <v>167</v>
-      </c>
-      <c r="M14" t="s">
-        <v>211</v>
-      </c>
-      <c r="N14" t="s">
-        <v>198</v>
-      </c>
-      <c r="O14" s="26">
-        <v>0</v>
-      </c>
-      <c r="P14" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="R14">
-        <v>3</v>
-      </c>
-      <c r="S14">
-        <v>75</v>
-      </c>
-      <c r="T14">
-        <v>50</v>
-      </c>
-      <c r="U14">
-        <v>60</v>
-      </c>
-      <c r="V14" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>10</v>
-      </c>
-      <c r="Y14" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z14" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="AA14" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AB14" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AC14" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AD14" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE14" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AF14" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI14" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="AJ14">
-        <v>30</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL14">
-        <v>5</v>
-      </c>
-      <c r="AM14">
-        <v>200</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AO14">
-        <v>1</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AQ14" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AR14">
-        <v>200</v>
-      </c>
-      <c r="AS14" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AT14" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AU14" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AV14" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AW14" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AY14" s="18" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -9543,7 +9397,7 @@
         <v>498</v>
       </c>
       <c r="C38" s="67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="67" t="b">
         <v>0</v>
@@ -18652,6 +18506,161 @@
         <v>0</v>
       </c>
     </row>
+    <row r="111" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>502</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C111" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D111" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>207</v>
+      </c>
+      <c r="F111" t="s">
+        <v>184</v>
+      </c>
+      <c r="G111">
+        <v>1000</v>
+      </c>
+      <c r="H111">
+        <v>500</v>
+      </c>
+      <c r="I111" t="s">
+        <v>109</v>
+      </c>
+      <c r="J111" t="s">
+        <v>109</v>
+      </c>
+      <c r="K111" t="s">
+        <v>204</v>
+      </c>
+      <c r="L111" t="s">
+        <v>167</v>
+      </c>
+      <c r="M111" t="s">
+        <v>211</v>
+      </c>
+      <c r="N111" t="s">
+        <v>198</v>
+      </c>
+      <c r="O111" s="26">
+        <v>0</v>
+      </c>
+      <c r="P111" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="R111">
+        <v>3</v>
+      </c>
+      <c r="S111">
+        <v>75</v>
+      </c>
+      <c r="T111">
+        <v>50</v>
+      </c>
+      <c r="U111">
+        <v>60</v>
+      </c>
+      <c r="V111" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="W111">
+        <v>0</v>
+      </c>
+      <c r="X111">
+        <v>10</v>
+      </c>
+      <c r="Y111" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z111" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="AA111" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AB111" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AC111" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AD111" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE111" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AF111" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AG111" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH111" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI111" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ111">
+        <v>30</v>
+      </c>
+      <c r="AK111" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL111">
+        <v>5</v>
+      </c>
+      <c r="AM111">
+        <v>200</v>
+      </c>
+      <c r="AN111" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO111">
+        <v>1</v>
+      </c>
+      <c r="AP111" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AQ111" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AR111">
+        <v>200</v>
+      </c>
+      <c r="AS111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT111" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AU111" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AV111" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AW111" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX111" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY111" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="AP4:AR4"/>
@@ -18667,82 +18676,82 @@
     <mergeCell ref="I4:K4"/>
   </mergeCells>
   <dataValidations xWindow="1269" yWindow="762" count="21">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN105:AN109 AN13:AN102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN105:AN109 AN13 AN111 AN15:AN102">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI9 AI105:AI109 AI13:AI102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI9 AI105:AI109 AI13 AI111 AI15:AI102">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH105:AH109 AH13:AH102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH105:AH109 AH13 AH111 AH15:AH102">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS6:AS9 AS105:AS109 AS13:AS102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS6:AS9 AS105:AS109 AS13 AS111 AS15:AS102">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P9 C6:D10 P105:P109 C105:D109 P13:P102 C13:D102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P9 C6:D10 P105:P109 C105:D109 C111:D111 C13:D13 C15:D102 P13 P111 P15:P102">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AB6:AB9 V6:V9 V105:V109 AB105:AB109 V13:V102 AB13:AB102">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AB6:AB9 V6:V9 V105:V109 AB105:AB109 AB13 AB111 AB15:AB102 V13 V111 V15:V102">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W6:X9 W105:X109 W13:X102">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="W6:X9 W105:X109 W111:X111 W13:X13 W15:X102">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="Y6:AA9 AC6:AC9 AE6:AE9 AC61 AC97:AC102 AE105:AE109 Y105:AA109 AC13:AC50 Y13:AA102 AE13:AE102">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="Y6:AA9 AC6:AC9 AE6:AE9 AC61 AC97:AC102 AE105:AE109 Y105:AA109 AE13 AE111 AE15:AE102 Y111:AA111 Y13:AA13 Y15:AA102 AC13 AC111 AC15:AC50">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AJ6:AJ9 AJ105:AJ109 AJ13:AJ102">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AJ6:AJ9 AJ105:AJ109 AJ13 AJ111 AJ15:AJ102">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AT6:AU9 AT105:AU109 AT13:AU102">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AT6:AU9 AT105:AU109 AT111:AU111 AT13:AU13 AT15:AU102">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AV6:AV9 AV105:AV109 AV13:AV102">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AV6:AV9 AV105:AV109 AV13 AV111 AV15:AV102">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AF6:AF9 AF97:AF102 AF13:AF83">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AF6:AF9 AF97:AF102 AF13 AF111 AF15:AF83">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AL6:AL9 AL105:AL109 AL13:AL102">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AL6:AL9 AL105:AL109 AL13 AL111 AL15:AL102">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM105:AM109 AM13:AM102">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM105:AM109 AM13 AM111 AM15:AM102">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO105:AO109 AO13:AO102">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO105:AO109 AO13 AO111 AO15:AO102">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AD6:AD9 AD105:AD109 AD13:AD102"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW6:AY9 AW105:AY109 AW13:AY102">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AD6:AD9 AD105:AD109 AD111 AD13 AD15:AD102"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW6:AY9 AW105:AY109 AW111:AY111 AW13:AY13 AW15:AY102">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP105:AP109 AP13:AP102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP105:AP109 AP13 AP111 AP15:AP102">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ9 AQ105:AQ109 AQ13:AQ102">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ9 AQ105:AQ109 AQ13 AQ111 AQ15:AQ102">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="S6:S9 S105:S109 S13:S102">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="S6:S9 S105:S109 S13 S111 S15:S102">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:J9 I105:J109 I13:J102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:J9 I105:J109 I111:J111 I13:J13 I15:J102">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -18755,37 +18764,37 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L9 L105:L109 L13:L102</xm:sqref>
+          <xm:sqref>L6:L9 L105:L109 L13 L111 L15:L102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$64:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M9 M105:M109 M13:M102</xm:sqref>
+          <xm:sqref>M6:M9 M105:M109 M13 M111 M15:M102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$45:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F9 F105:F109 F13:F102</xm:sqref>
+          <xm:sqref>F6:F9 F105:F109 F13 F111 F15:F102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E9 E105:E109 E13:E102</xm:sqref>
+          <xm:sqref>E6:E9 E105:E109 E13 E111 E15:E102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:K9 K105:K109 K13:K102</xm:sqref>
+          <xm:sqref>K6:K9 K105:K109 K13 K111 K15:K102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$74:$A$77</xm:f>
           </x14:formula1>
-          <xm:sqref>N6:N9 N105:N109 N13:N102</xm:sqref>
+          <xm:sqref>N6:N9 N105:N109 N13 N111 N15:N102</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18803,7 +18812,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -18915,13 +18924,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.625"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -18991,10 +19000,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.375"/>
+    <col min="1" max="1" width="23.42578125"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.375"/>
-    <col min="4" max="1025" width="8.625"/>
+    <col min="3" max="3" width="85.42578125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -19403,11 +19412,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.875" style="31" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" style="31" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="110" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20053,11 +20062,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.125" customWidth="1"/>
-    <col min="2" max="2" width="25.25" customWidth="1"/>
-    <col min="3" max="3" width="54.875" customWidth="1"/>
-    <col min="4" max="4" width="72.25" customWidth="1"/>
-    <col min="5" max="5" width="36.25" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">

</xml_diff>